<commit_message>
Using mutex with parallel threading to avoid race condition and modularized code into different .cpp and .h files version 4.0
</commit_message>
<xml_diff>
--- a/order_book/runtime_optimisation_record_book.xlsx
+++ b/order_book/runtime_optimisation_record_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My works\Miscelleneous\Quant-finance\order_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B1398073-89A6-4803-B25D-1C72EE464E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CBE01B-DB13-4932-9968-7139F38AACF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="2676" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>version 1.0</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Using parallel processing and unordered_maps to take as many orders as possible together on simulateTrading and then print the status of order book only once in the end, to avoid race conditions</t>
+  </si>
+  <si>
+    <t>version 4.0</t>
+  </si>
+  <si>
+    <t>Using mutex to avoid race condition and modularized code into different .cpp and .h files</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,7 +320,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
@@ -624,7 +629,7 @@
   <dimension ref="B3:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -667,7 +672,7 @@
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="5">
@@ -691,7 +696,7 @@
       <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5">
@@ -807,10 +812,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>9017</v>
+      </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F12" si="1">E12/1000</f>
+        <v>9.0169999999999995</v>
       </c>
       <c r="K12" t="s">
         <v>13</v>
@@ -906,21 +923,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <TemplafyTemplateConfiguration><![CDATA[{"transformationConfigurations":[{"colorTheme":"{{DataSources.ColorThemes[\"Arup\"].ColorTheme}}","disableUpdates":false,"type":"colorTheme"}],"templateName":"Arup Blank","templateDescription":"","enableDocumentContentUpdater":false,"version":"2.0"}]]></TemplafyTemplateConfiguration>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<TemplafyFormConfiguration><![CDATA[{"formFields":[],"formDataEntries":[]}]]></TemplafyFormConfiguration>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59C169C-5B71-4139-B067-6BD7D31FA149}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62CB8C1F-D40D-4C86-BB4B-0CF96D922D6C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62CB8C1F-D40D-4C86-BB4B-0CF96D922D6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59C169C-5B71-4139-B067-6BD7D31FA149}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>